<commit_message>
Added annotations to the rate input sheet
Added automation and annotation to the rate input sheet to guide users. The sheet now automatically blacks-out cells that you do not need to populate based on the three key parameters of your rate structure asked at the top of the input sheet.
</commit_message>
<xml_diff>
--- a/apps/elpt/AllUploadFiles_ToolTesting/Rate Input Sheet.xlsx
+++ b/apps/elpt/AllUploadFiles_ToolTesting/Rate Input Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muham\Documents\GitHub\Archive\IAC-Decarb-Tools\apps\elpt\AllUploadFiles_ToolTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucdavis365-my.sharepoint.com/personal/mqamar_ucdavis_edu/Documents/Documents/GitHub/IAC-Decarb-Tools/apps/elpt/AllUploadFiles_ToolTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC43E3EC-AF8F-4D01-9B80-4282726D8A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{25E5316F-A62E-451D-80F3-6B5B67DB1A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{E370F02F-D469-4C37-87C0-D114AE20DC81}"/>
+    <workbookView xWindow="11350" yWindow="3840" windowWidth="21640" windowHeight="16280" xr2:uid="{E370F02F-D469-4C37-87C0-D114AE20DC81}"/>
   </bookViews>
   <sheets>
     <sheet name="Rate Inputs" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,50 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>M Ali Qamar</author>
+  </authors>
+  <commentList>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{B85FD35E-EF49-4818-BE5B-C8355A589474}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Tip:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Once you fill in these three key parameters of your rate structure, this input sheet will automatically black-out all the cells you do not need to populate. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
   <si>
@@ -178,7 +222,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h\ AM/PM"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,8 +267,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,12 +318,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -474,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -542,15 +599,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -568,17 +616,70 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF07245D"/>
       <color rgb="FF8FCEE5"/>
-      <color rgb="FF07245D"/>
     </mruColors>
   </colors>
   <extLst>
@@ -908,29 +1009,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA68E0AC-8D3D-4CCA-853C-25AF0E85BA11}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA68E0AC-8D3D-4CCA-853C-25AF0E85BA11}">
   <dimension ref="B2:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="38.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6328125" style="1"/>
+    <col min="2" max="2" width="38.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" style="1" customWidth="1"/>
     <col min="5" max="13" width="18.6328125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="1"/>
+    <col min="14" max="16384" width="8.6328125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="2:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="32" t="s">
         <v>43</v>
       </c>
       <c r="F3" s="4"/>
@@ -970,7 +1071,7 @@
       <c r="D10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="29" t="s">
         <v>40</v>
       </c>
     </row>
@@ -981,7 +1082,7 @@
       <c r="D11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="33"/>
+      <c r="F11" s="30"/>
     </row>
     <row r="12" spans="2:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="2:8" s="5" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1005,22 +1106,22 @@
       </c>
     </row>
     <row r="14" spans="2:8" s="4" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C14" s="28">
+      <c r="C14" s="25">
         <v>0.875</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="26">
         <v>0.58333333333333304</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="25">
         <v>0.58333333333333304</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="25">
         <v>0.66666666666666696</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="26">
         <v>0.66666666666666696</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="27">
         <v>0.875</v>
       </c>
     </row>
@@ -1088,13 +1189,13 @@
     </row>
     <row r="19" spans="2:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="20" spans="2:8" s="2" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="31"/>
+      <c r="D20" s="28"/>
     </row>
     <row r="21" spans="2:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="33">
+      <c r="B21" s="30">
         <v>40</v>
       </c>
     </row>
@@ -1112,20 +1213,20 @@
       <c r="D25" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F25" s="32" t="s">
+      <c r="F25" s="29" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C26" s="26" t="str">
+      <c r="C26" s="17" t="str">
         <f>TEXT(DATE(2025, MATCH(D11, {"January","February","March","April","May","June","July","August","September","October","November","December"},0)+1, 1), "MMMM")</f>
         <v>October</v>
       </c>
-      <c r="D26" s="27" t="str">
+      <c r="D26" s="19" t="str">
         <f>TEXT(DATE(2025, MATCH(C11, {"January","February","March","April","May","June","July","August","September","October","November","December"},0)-1, 1), "MMMM")</f>
         <v>March</v>
       </c>
-      <c r="F26" s="33"/>
+      <c r="F26" s="30"/>
     </row>
     <row r="27" spans="2:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="28" spans="2:8" s="5" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1149,22 +1250,22 @@
       </c>
     </row>
     <row r="29" spans="2:8" s="4" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C29" s="28">
+      <c r="C29" s="25">
         <v>0.875</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="26">
         <v>0.58333333333333304</v>
       </c>
-      <c r="E29" s="29">
+      <c r="E29" s="26">
         <v>0.58333333333333304</v>
       </c>
-      <c r="F29" s="29">
+      <c r="F29" s="26">
         <v>0.66666666666666696</v>
       </c>
-      <c r="G29" s="29">
+      <c r="G29" s="26">
         <v>0.66666666666666696</v>
       </c>
-      <c r="H29" s="30">
+      <c r="H29" s="27">
         <v>0.875</v>
       </c>
     </row>
@@ -1232,13 +1333,13 @@
     </row>
     <row r="34" spans="2:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="35" spans="2:8" s="2" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="31"/>
+      <c r="D35" s="28"/>
     </row>
     <row r="36" spans="2:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="33">
+      <c r="B36" s="30">
         <v>35</v>
       </c>
     </row>
@@ -1258,7 +1359,39 @@
     <row r="50" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="51" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
+  <conditionalFormatting sqref="B21 B36">
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>$C$5&lt;&gt;"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18 E18 G18 C33 E33 G33">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>$C$3="Only Demand Charge ($/kW)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:D14 G14:H14 C18:D18 G18:H18 C29:D29 G29:H29 C33:D33 G33:H33">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$C$3="Fixed Usage and Demand Charges"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18 F18 H18 D33 F33 H33">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$C$3="Only Usage Charge ($/kWh)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:F18 E33:F33 E14:F14 E29:F29">
+    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
+      <formula>OR($C$4="No", $C$3="Fixed Usage and Demand Charges")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11 F26">
+    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
+      <formula>$C$3&lt;&gt;"Fixed Usage and Demand Charges"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
@@ -1300,7 +1433,7 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="18.1796875" customWidth="1"/>
   </cols>

</xml_diff>